<commit_message>
addr query deploying v20211213.
</commit_message>
<xml_diff>
--- a/lnglat/sample.xlsx
+++ b/lnglat/sample.xlsx
@@ -1,41 +1,35 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24701"/>
+  <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\MapC\lnglat\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\MapC\lnglat\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1FDA433E-7818-43A5-B246-BFAC5778CB10}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="195" windowWidth="25440" windowHeight="15540"/>
+    <workbookView xWindow="14835" yWindow="3030" windowWidth="21600" windowHeight="11505" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="qh" localSheetId="0">Sheet1!$A$2:$A$2582</definedName>
+    <definedName name="qh" localSheetId="0">Sheet1!$A$3:$A$2582</definedName>
   </definedNames>
   <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/connections.xml><?xml version="1.0" encoding="utf-8"?>
-<connections xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <connection id="1" name="qh" type="6" refreshedVersion="7" background="1" saveData="1">
+<connections xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16">
+  <connection id="1" xr16:uid="{00000000-0015-0000-FFFF-FFFF00000000}" name="qh" type="6" refreshedVersion="7" background="1" saveData="1">
     <textPr codePage="936" sourceFile="D:\ymy\qh\qh.txt" comma="1">
       <textFields count="2">
         <textField/>
@@ -47,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
   <si>
     <t>地址</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -60,11 +54,31 @@
     <t>上海市正大广场</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
+  <si>
+    <t>上海豫园</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>东方明珠电视塔</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>上海中心大厦</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>一大会址</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>南浦大桥</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -126,7 +140,7 @@
 </file>
 
 <file path=xl/queryTables/queryTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="qh" connectionId="1" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="qh" connectionId="1" xr16:uid="{00000000-0016-0000-0000-000000000000}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -425,11 +439,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:A3"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:A8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -444,11 +458,36 @@
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>1</v>
+        <v>6</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
         <v>2</v>
       </c>
     </row>

</xml_diff>